<commit_message>
Updates to sail data and strings
</commit_message>
<xml_diff>
--- a/sail_data.xlsx
+++ b/sail_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JackPreece\Code\Test scripts\for_fun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02229DBB-C68E-4A83-98D8-8AACE5B63554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{BB3803EE-8037-4517-AA7D-9AF8EA30A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="14">
   <si>
     <t>J1</t>
   </si>
@@ -125,7 +125,187 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1023,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1281,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1163,49 +1343,49 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
       <c r="M3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="P3" t="s">
         <v>7</v>
@@ -1225,22 +1405,22 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -1287,7 +1467,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1305,51 +1485,51 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="T5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -1376,22 +1556,22 @@
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="P6" t="s">
         <v>4</v>
@@ -1411,69 +1591,176 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" t="s">
-        <v>2</v>
-      </c>
-      <c r="S7" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B2:T7">
+  <conditionalFormatting sqref="B3:T8">
+    <cfRule type="cellIs" dxfId="32" priority="13" operator="equal">
+      <formula>"A1"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="S1">
+      <formula>NOT(ISERROR(SEARCH("S1",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="S3">
+      <formula>NOT(ISERROR(SEARCH("S3",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="S2">
+      <formula>NOT(ISERROR(SEARCH("S2",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="17" operator="containsText" text="S4">
+      <formula>NOT(ISERROR(SEARCH("S4",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="code zero">
+      <formula>NOT(ISERROR(SEARCH("code zero",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="J2">
+      <formula>NOT(ISERROR(SEARCH("J2",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="J1">
+      <formula>NOT(ISERROR(SEARCH("J1",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="J3">
+      <formula>NOT(ISERROR(SEARCH("J3",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="J2">
+      <formula>NOT(ISERROR(SEARCH("J2",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="J1">
+      <formula>NOT(ISERROR(SEARCH("J1",B3)))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:T2">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"A1"</formula>
     </cfRule>

</xml_diff>